<commit_message>
acdom is now absorption to be consistent with the complete cdom profiles data
</commit_message>
<xml_diff>
--- a/dataset/raw/literature/hernes2008/data.xlsx
+++ b/dataset/raw/literature/hernes2008/data.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">doc</t>
   </si>
   <si>
-    <t xml:space="preserve">acdom</t>
+    <t xml:space="preserve">absorption</t>
   </si>
   <si>
     <t xml:space="preserve">wavelength</t>
@@ -168,19 +168,19 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8391608391608"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.47552447552448"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.58741258741259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.027972027972"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.25174825174825"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.32867132867133"/>
-    <col collapsed="false" hidden="false" max="1021" min="7" style="1" width="14.6153846153846"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="14.6153846153846"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.2867132867133"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.10489510489511"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.21678321678322"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4685314685315"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.88111888111888"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.95804195804196"/>
+    <col collapsed="false" hidden="false" max="1021" min="7" style="1" width="14.0629370629371"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="14.0629370629371"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>